<commit_message>
finished with results 1/2
</commit_message>
<xml_diff>
--- a/java/out/production/java/results/Inst1_Ord_80_Veh_45_Loc_45_OPERATOR_ANALYSIS_EXTRA.xlsx
+++ b/java/out/production/java/results/Inst1_Ord_80_Veh_45_Loc_45_OPERATOR_ANALYSIS_EXTRA.xlsx
@@ -184,11 +184,12 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -210,9 +211,15 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -221,14 +228,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCCCCCC"/>
-        <bgColor rgb="FFCCCCFF"/>
+        <fgColor rgb="FF72BF44"/>
+        <bgColor rgb="FF339966"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF666699"/>
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB2B2B2"/>
+        <bgColor rgb="FFB3B3B3"/>
       </patternFill>
     </fill>
   </fills>
@@ -266,7 +279,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -279,15 +292,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -316,7 +349,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFCCCCCC"/>
+      <rgbColor rgb="FFB3B3B3"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -325,7 +358,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -344,12 +377,12 @@
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF72BF44"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF420E"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FFB3B3B3"/>
+      <rgbColor rgb="FFB2B2B2"/>
       <rgbColor rgb="FF004586"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -390,6 +423,8 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -627,6 +662,8 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -741,17 +778,17 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="36009544"/>
-        <c:axId val="88580731"/>
+        <c:axId val="17359908"/>
+        <c:axId val="10239055"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="36009544"/>
+        <c:axId val="17359908"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="@" sourceLinked="1"/>
+        <c:numFmt formatCode="@" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -773,12 +810,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88580731"/>
+        <c:crossAx val="10239055"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="88580731"/>
+        <c:axId val="10239055"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="65000"/>
@@ -794,7 +831,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -816,7 +853,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36009544"/>
+        <c:crossAx val="17359908"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -875,9 +912,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>719280</xdr:colOff>
+      <xdr:colOff>718920</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>105480</xdr:rowOff>
+      <xdr:rowOff>105120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -885,8 +922,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9242280" y="1415160"/>
-        <a:ext cx="5752800" cy="3241800"/>
+        <a:off x="9240840" y="1415160"/>
+        <a:ext cx="5752800" cy="3241440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -907,7 +944,7 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -916,7 +953,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.14"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -1316,10 +1353,10 @@
       <c r="B19" s="0" t="n">
         <v>6422128.60039654</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="C19" s="3" t="n">
         <v>21317.0482146229</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="3" t="n">
         <v>20593.1833904361</v>
       </c>
       <c r="E19" s="0" t="n">
@@ -1394,29 +1431,29 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="0" t="n">
-        <v>6422128.60039654</v>
-      </c>
-      <c r="C22" s="0" t="n">
+      <c r="B22" s="5" t="n">
+        <v>6422128.60039654</v>
+      </c>
+      <c r="C22" s="5" t="n">
         <v>21472.8051512056</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="D22" s="5" t="n">
         <v>20826.5294082723</v>
       </c>
-      <c r="E22" s="0" t="n">
+      <c r="E22" s="5" t="n">
         <v>0.03009740638833</v>
       </c>
-      <c r="F22" s="0" t="n">
+      <c r="F22" s="5" t="n">
         <v>20.1631763377</v>
       </c>
-      <c r="G22" s="2" t="n">
+      <c r="G22" s="6" t="n">
         <f aca="false">+($C$38-C22)/$C$38</f>
         <v>-0.00506762029806587</v>
       </c>
-      <c r="H22" s="2" t="n">
+      <c r="H22" s="6" t="n">
         <f aca="false">+($D$38-D22)/$D$38</f>
         <v>-0.00559991001606514</v>
       </c>
@@ -1618,29 +1655,29 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="0" t="n">
-        <v>6422128.60039654</v>
-      </c>
-      <c r="C30" s="0" t="n">
+      <c r="B30" s="5" t="n">
+        <v>6422128.60039654</v>
+      </c>
+      <c r="C30" s="5" t="n">
         <v>21705.7139762399</v>
       </c>
-      <c r="D30" s="0" t="n">
+      <c r="D30" s="5" t="n">
         <v>20842.0783335733</v>
       </c>
-      <c r="E30" s="0" t="n">
+      <c r="E30" s="5" t="n">
         <v>0.0397884005848401</v>
       </c>
-      <c r="F30" s="0" t="n">
+      <c r="F30" s="5" t="n">
         <v>13.3042604661</v>
       </c>
-      <c r="G30" s="2" t="n">
+      <c r="G30" s="6" t="n">
         <f aca="false">+($C$38-C30)/$C$38</f>
         <v>-0.0159692755254686</v>
       </c>
-      <c r="H30" s="2" t="n">
+      <c r="H30" s="6" t="n">
         <f aca="false">+($D$38-D30)/$D$38</f>
         <v>-0.00635068310825798</v>
       </c>
@@ -1730,29 +1767,29 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="0" t="n">
-        <v>6422128.60039654</v>
-      </c>
-      <c r="C34" s="0" t="n">
+      <c r="B34" s="5" t="n">
+        <v>6422128.60039654</v>
+      </c>
+      <c r="C34" s="5" t="n">
         <v>22551.2264391159</v>
       </c>
-      <c r="D34" s="0" t="n">
+      <c r="D34" s="5" t="n">
         <v>20668.4697069062</v>
       </c>
-      <c r="E34" s="0" t="n">
+      <c r="E34" s="5" t="n">
         <v>0.0834879973066111</v>
       </c>
-      <c r="F34" s="0" t="n">
+      <c r="F34" s="5" t="n">
         <v>20.0823706511</v>
       </c>
-      <c r="G34" s="2" t="n">
+      <c r="G34" s="6" t="n">
         <f aca="false">+($C$38-C34)/$C$38</f>
         <v>-0.055544784780601</v>
       </c>
-      <c r="H34" s="2" t="n">
+      <c r="H34" s="6" t="n">
         <f aca="false">+($D$38-D34)/$D$38</f>
         <v>0.00203193388624921</v>
       </c>
@@ -1786,85 +1823,85 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B36" s="0" t="n">
-        <v>6422128.60039654</v>
-      </c>
-      <c r="C36" s="0" t="n">
+      <c r="B36" s="5" t="n">
+        <v>6422128.60039654</v>
+      </c>
+      <c r="C36" s="5" t="n">
         <v>21377.0583806266</v>
       </c>
-      <c r="D36" s="0" t="n">
+      <c r="D36" s="5" t="n">
         <v>20910.641425186</v>
       </c>
-      <c r="E36" s="0" t="n">
+      <c r="E36" s="5" t="n">
         <v>0.021818575181667</v>
       </c>
-      <c r="F36" s="0" t="n">
+      <c r="F36" s="5" t="n">
         <v>21.6820045964</v>
       </c>
-      <c r="G36" s="2" t="n">
+      <c r="G36" s="6" t="n">
         <f aca="false">+($C$38-C36)/$C$38</f>
         <v>-0.000586045665437057</v>
       </c>
-      <c r="H36" s="2" t="n">
+      <c r="H36" s="6" t="n">
         <f aca="false">+($D$38-D36)/$D$38</f>
         <v>-0.00966122215221492</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B37" s="0" t="n">
-        <v>6422128.60039654</v>
-      </c>
-      <c r="C37" s="0" t="n">
+      <c r="B37" s="5" t="n">
+        <v>6422128.60039654</v>
+      </c>
+      <c r="C37" s="5" t="n">
         <v>21439.81287569</v>
       </c>
-      <c r="D37" s="0" t="n">
+      <c r="D37" s="5" t="n">
         <v>20958.8397733332</v>
       </c>
-      <c r="E37" s="0" t="n">
+      <c r="E37" s="5" t="n">
         <v>0.0224336427349227</v>
       </c>
-      <c r="F37" s="0" t="n">
+      <c r="F37" s="5" t="n">
         <v>19.5652018373</v>
       </c>
-      <c r="G37" s="2" t="n">
+      <c r="G37" s="6" t="n">
         <f aca="false">+($C$38-C37)/$C$38</f>
         <v>-0.00352336617722906</v>
       </c>
-      <c r="H37" s="2" t="n">
+      <c r="H37" s="6" t="n">
         <f aca="false">+($D$38-D37)/$D$38</f>
         <v>-0.0119884584194553</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B38" s="0" t="n">
-        <v>6422128.60039654</v>
-      </c>
-      <c r="C38" s="0" t="n">
+      <c r="B38" s="9" t="n">
+        <v>6422128.60039654</v>
+      </c>
+      <c r="C38" s="9" t="n">
         <v>21364.5377858631</v>
       </c>
-      <c r="D38" s="0" t="n">
+      <c r="D38" s="9" t="n">
         <v>20710.5521796831</v>
       </c>
-      <c r="E38" s="0" t="n">
+      <c r="E38" s="9" t="n">
         <v>0.0306108006049544</v>
       </c>
-      <c r="F38" s="0" t="n">
+      <c r="F38" s="9" t="n">
         <v>18.4493458595</v>
       </c>
-      <c r="G38" s="2" t="n">
+      <c r="G38" s="10" t="n">
         <f aca="false">+($C$38-C38)/$C$38</f>
         <v>0</v>
       </c>
-      <c r="H38" s="2" t="n">
+      <c r="H38" s="10" t="n">
         <f aca="false">+($D$38-D38)/$D$38</f>
         <v>0</v>
       </c>

</xml_diff>